<commit_message>
Nhập toàn bộ thông tin của lớp sinh hoạt vào file "Phan Nhiem.xlsx"
</commit_message>
<xml_diff>
--- a/2013/Phan Nhiem.xlsx
+++ b/2013/Phan Nhiem.xlsx
@@ -4,12 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="435" windowWidth="19875" windowHeight="7710"/>
+    <workbookView xWindow="480" yWindow="435" windowWidth="19875" windowHeight="7710" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Thong tin" sheetId="5" r:id="rId1"/>
     <sheet name="Co cau" sheetId="2" r:id="rId2"/>
-    <sheet name="Phan nhiem" sheetId="1" r:id="rId3"/>
+    <sheet name="Nhom chuyen mon" sheetId="1" r:id="rId3"/>
+    <sheet name="Lich sinh hoat" sheetId="6" r:id="rId4"/>
+    <sheet name="Phan cong truc" sheetId="7" r:id="rId5"/>
+    <sheet name="Danh sach" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="ThongTinBDH">'Thong tin'!$E$4:$E$28</definedName>
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="240">
   <si>
     <t>Hành chánh</t>
   </si>
@@ -177,27 +180,6 @@
     <t>Soài</t>
   </si>
   <si>
-    <t>Trưởng trực</t>
-  </si>
-  <si>
-    <t>Giữ xe</t>
-  </si>
-  <si>
-    <t>Chia vị trí</t>
-  </si>
-  <si>
-    <t>Nắm bắt chương trình trong tháng</t>
-  </si>
-  <si>
-    <t>Nhắc nhở, đôn đốc những anh chị có nhiệm vụ trong tháng</t>
-  </si>
-  <si>
-    <t>Hỗ trợ ban phụng vụ chầu cuối tháng</t>
-  </si>
-  <si>
-    <t>Phụ trách chính sinh hoạt đầu tháng</t>
-  </si>
-  <si>
     <t>Giuse Đinh Trường Trúc Giang</t>
   </si>
   <si>
@@ -420,79 +402,7 @@
     <t>Maria Bùi Thị Yến Nhi</t>
   </si>
   <si>
-    <t>Vicente Vũ Văn Bảo</t>
-  </si>
-  <si>
-    <t>Anna Phạm Lê Uyên Nhi</t>
-  </si>
-  <si>
-    <t>Giuse Nguyễn Minh Tân</t>
-  </si>
-  <si>
-    <t>Giuse Bùi Quang Phúc</t>
-  </si>
-  <si>
-    <t>Phero Lê Thanh Thiên</t>
-  </si>
-  <si>
-    <t>Teresa Hà Tôn Nữ TràMy</t>
-  </si>
-  <si>
-    <t>Phero Vũ Văn An</t>
-  </si>
-  <si>
-    <t>Teresa Nguyễn Hồng Hạnh</t>
-  </si>
-  <si>
-    <t>Giuse Nguyễn Thiên Long</t>
-  </si>
-  <si>
-    <t>Maria Giuse Vũ Thị Thủy Tiên</t>
-  </si>
-  <si>
-    <t>Giuse Phạm Quốc Sơn</t>
-  </si>
-  <si>
-    <t>Phero Trần Đức Duy</t>
-  </si>
-  <si>
-    <t>Đaminh Phạm Minh Đức</t>
-  </si>
-  <si>
-    <t>Teresa Phạm Vũ Thúy Ngọc</t>
-  </si>
-  <si>
-    <t>Giuse Nguyễn Tấn Duy</t>
-  </si>
-  <si>
-    <t>Maria Đỗ Thị Hiền</t>
-  </si>
-  <si>
-    <t>Phaolo Nguyễn Mạnh Công</t>
-  </si>
-  <si>
-    <t>Teresa Trần Minh Trân</t>
-  </si>
-  <si>
-    <t>Giuse Nguyễn Phú Nguyên</t>
-  </si>
-  <si>
-    <t>Catarina Bùi Thị Hồng Trâm</t>
-  </si>
-  <si>
     <t>Vicente Nguyễn Văn Ngà</t>
-  </si>
-  <si>
-    <t>Vicente Vũ Văn Long</t>
-  </si>
-  <si>
-    <t>Anna Nguyễn Thị Hoài Nam</t>
-  </si>
-  <si>
-    <t>Anton Trần Phước Hợp</t>
-  </si>
-  <si>
-    <t>Maria Bùi Thị Ngọc Nữ</t>
   </si>
   <si>
     <t>Ngày sinh</t>
@@ -677,17 +587,239 @@
   </si>
   <si>
     <t>clovernguyen25@gmail.com</t>
+  </si>
+  <si>
+    <t>Tháng</t>
+  </si>
+  <si>
+    <t>Cấp 1</t>
+  </si>
+  <si>
+    <t>Cấp 2</t>
+  </si>
+  <si>
+    <t>Đội trưởng</t>
+  </si>
+  <si>
+    <t>Ghi chú</t>
+  </si>
+  <si>
+    <t>Nghiêm tập</t>
+  </si>
+  <si>
+    <t>Sổ sách, hành chánh</t>
+  </si>
+  <si>
+    <t>Học chung</t>
+  </si>
+  <si>
+    <t>Bài hát phong trào</t>
+  </si>
+  <si>
+    <t>Họp đội</t>
+  </si>
+  <si>
+    <t>Lãnh nhận lời Chúa</t>
+  </si>
+  <si>
+    <t>Hoa thiêng Thánh Thể</t>
+  </si>
+  <si>
+    <t>Cầu nguyện</t>
+  </si>
+  <si>
+    <t>Giờ Thánh Thể</t>
+  </si>
+  <si>
+    <t>Morse (giới thiệu)</t>
+  </si>
+  <si>
+    <t>Morse (thổi)</t>
+  </si>
+  <si>
+    <t>Mật thư</t>
+  </si>
+  <si>
+    <t>Mật thư Thánh Kinh</t>
+  </si>
+  <si>
+    <t>Nút dây</t>
+  </si>
+  <si>
+    <t>Dấu đường</t>
+  </si>
+  <si>
+    <t>Dựng lều</t>
+  </si>
+  <si>
+    <t>Sermaphore</t>
+  </si>
+  <si>
+    <t>Phân đội</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>IV</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>PHÂN CÔNG TRỰC CÁC THÁNG</t>
+  </si>
+  <si>
+    <t>CHƯƠNG TRÌNH SINH HOẠT NIÊN KHÓA 2012-2013</t>
+  </si>
+  <si>
+    <t>Vicente
+Vũ Văn Bảo</t>
+  </si>
+  <si>
+    <t>Anna
+Phạm Lê Uyên Nhi</t>
+  </si>
+  <si>
+    <t>Giuse
+Nguyễn Minh Tân</t>
+  </si>
+  <si>
+    <t>Giuse
+Bùi Quang Phúc</t>
+  </si>
+  <si>
+    <t>Phero
+Lê Thanh Thiên</t>
+  </si>
+  <si>
+    <t>Teresa
+Hà Tôn Nữ Trà My</t>
+  </si>
+  <si>
+    <t>Phero
+Vũ Văn An</t>
+  </si>
+  <si>
+    <t>Teresa
+Nguyễn Hồng Hạnh</t>
+  </si>
+  <si>
+    <t>Giuse
+Nguyễn Thiên Long</t>
+  </si>
+  <si>
+    <t>Vicente
+Vũ Văn Long</t>
+  </si>
+  <si>
+    <t>Giuse
+Phạm Quốc Sơn</t>
+  </si>
+  <si>
+    <t>Phero
+Vũ Đức Duy</t>
+  </si>
+  <si>
+    <t>Maria Giuse
+Vũ Thị Thủy Tiên</t>
+  </si>
+  <si>
+    <t>Đaminh
+Phạm Minh Đức</t>
+  </si>
+  <si>
+    <t>Teresa
+Phạm Vũ Thúy Ngọc</t>
+  </si>
+  <si>
+    <t>Maria
+Đỗ Thị Hiền</t>
+  </si>
+  <si>
+    <t>Giuse
+Nguyễn Tấn Duy</t>
+  </si>
+  <si>
+    <t>Phaolo
+Nguyễn Mạnh Công</t>
+  </si>
+  <si>
+    <t>Teresa
+Trần Minh Trân</t>
+  </si>
+  <si>
+    <t>Giuse
+Nguyễn Phú Nguyên</t>
+  </si>
+  <si>
+    <t>Catarina
+Bùi Thị Hồng Trâm</t>
+  </si>
+  <si>
+    <t>Anna
+Nguyễn Thị Hoài Nam</t>
+  </si>
+  <si>
+    <t>Maria
+Bùi Thị Ngọc Nữ</t>
+  </si>
+  <si>
+    <t>Anton
+Trần Phước Hợp</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Nhiệm vụ phân đội trực:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+- Làm trưởng trực các tối thức 5 và các ngày học đội trưởng (nếu cần).
+- Phân công giữ xe.
+- Nắm chương trình dạy của tháng, liên lạc với các ban liên quan biết cần phải chuẩn bị những gì cho buổi học.
+- Liên hệ với các ban quản lý, kỹ thuật, hành chánh… nếu cần thiết để đảm bảo các buổi học được chuẩn bị đầy đủ.
+- Điều phối chương trình sinh hoạt trong tháng.
+- Chuẩn bị giờ chầu cuối tháng.
+- Lên kế hoạch chương trình sinh hoạt đầu tháng (trò chơi vân động, hành trình sa mạc…) và phổ biến cho các anh chị khác.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="dd\-mm"/>
+    <numFmt numFmtId="166" formatCode="dd/mm"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -772,6 +904,20 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -829,7 +975,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -975,11 +1121,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalDown="1">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal style="thin">
+        <color auto="1"/>
+      </diagonal>
+    </border>
+    <border diagonalDown="1">
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal style="thin">
+        <color auto="1"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1045,77 +1215,132 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="lightDown">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1414,8 +1639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,49 +1659,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
-        <v>159</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="A1" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>153</v>
+        <v>122</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>154</v>
+        <v>123</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>155</v>
+        <v>124</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>173</v>
+        <v>142</v>
       </c>
       <c r="J3" s="30" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1484,10 +1709,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D4" s="25" t="s">
         <v>31</v>
@@ -1503,7 +1728,7 @@
         <v>40987</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>174</v>
+        <v>143</v>
       </c>
       <c r="I4" s="25"/>
       <c r="J4" s="31"/>
@@ -1513,10 +1738,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D5" s="25" t="s">
         <v>24</v>
@@ -1532,13 +1757,13 @@
         <v>41183</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>175</v>
+        <v>144</v>
       </c>
       <c r="I5" s="25" t="s">
-        <v>200</v>
+        <v>169</v>
       </c>
       <c r="J5" s="33" t="s">
-        <v>205</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1546,10 +1771,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D6" s="25" t="s">
         <v>25</v>
@@ -1565,13 +1790,13 @@
         <v>41183</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>176</v>
+        <v>145</v>
       </c>
       <c r="I6" s="25" t="s">
-        <v>201</v>
+        <v>170</v>
       </c>
       <c r="J6" s="33" t="s">
-        <v>206</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1579,10 +1804,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D7" s="25" t="s">
         <v>28</v>
@@ -1598,7 +1823,7 @@
         <v>41160</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>177</v>
+        <v>146</v>
       </c>
       <c r="I7" s="25"/>
       <c r="J7" s="31"/>
@@ -1608,10 +1833,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D8" s="25" t="s">
         <v>23</v>
@@ -1627,13 +1852,13 @@
         <v>41181</v>
       </c>
       <c r="H8" s="28" t="s">
-        <v>178</v>
+        <v>147</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>195</v>
+        <v>164</v>
       </c>
       <c r="J8" s="33" t="s">
-        <v>207</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1641,10 +1866,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D9" s="25" t="s">
         <v>43</v>
@@ -1660,11 +1885,11 @@
         <v>41237</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>179</v>
+        <v>148</v>
       </c>
       <c r="I9" s="25"/>
       <c r="J9" s="33" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1672,10 +1897,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D10" s="25" t="s">
         <v>42</v>
@@ -1691,13 +1916,13 @@
         <v>40987</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="I10" s="25" t="s">
-        <v>157</v>
+        <v>126</v>
       </c>
       <c r="J10" s="33" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1705,10 +1930,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D11" s="25" t="s">
         <v>42</v>
@@ -1724,11 +1949,11 @@
         <v>41116</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>177</v>
+        <v>146</v>
       </c>
       <c r="I11" s="25"/>
       <c r="J11" s="33" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1736,13 +1961,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E12" s="25" t="str">
         <f t="shared" si="0"/>
@@ -1753,11 +1978,11 @@
       </c>
       <c r="G12" s="27"/>
       <c r="H12" s="28" t="s">
-        <v>180</v>
+        <v>149</v>
       </c>
       <c r="I12" s="25"/>
       <c r="J12" s="33" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1765,10 +1990,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D13" s="25" t="s">
         <v>39</v>
@@ -1786,7 +2011,7 @@
       <c r="H13" s="28"/>
       <c r="I13" s="25"/>
       <c r="J13" s="33" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1794,10 +2019,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D14" s="25" t="s">
         <v>39</v>
@@ -1814,10 +2039,10 @@
       </c>
       <c r="H14" s="28"/>
       <c r="I14" s="25" t="s">
-        <v>202</v>
+        <v>171</v>
       </c>
       <c r="J14" s="33" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1825,10 +2050,10 @@
         <v>12</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D15" s="25" t="s">
         <v>39</v>
@@ -1844,13 +2069,13 @@
         <v>41089</v>
       </c>
       <c r="H15" s="28" t="s">
-        <v>181</v>
+        <v>150</v>
       </c>
       <c r="I15" s="25" t="s">
-        <v>203</v>
+        <v>172</v>
       </c>
       <c r="J15" s="33" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1858,10 +2083,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D16" s="25" t="s">
         <v>44</v>
@@ -1877,7 +2102,7 @@
         <v>41160</v>
       </c>
       <c r="H16" s="28" t="s">
-        <v>182</v>
+        <v>151</v>
       </c>
       <c r="I16" s="25"/>
       <c r="J16" s="33"/>
@@ -1887,10 +2112,10 @@
         <v>14</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D17" s="25" t="s">
         <v>41</v>
@@ -1906,13 +2131,13 @@
         <v>41183</v>
       </c>
       <c r="H17" s="28" t="s">
-        <v>183</v>
+        <v>152</v>
       </c>
       <c r="I17" s="25" t="s">
-        <v>196</v>
+        <v>165</v>
       </c>
       <c r="J17" s="33" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1920,10 +2145,10 @@
         <v>15</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D18" s="25" t="s">
         <v>46</v>
@@ -1939,7 +2164,7 @@
         <v>41030</v>
       </c>
       <c r="H18" s="28" t="s">
-        <v>184</v>
+        <v>153</v>
       </c>
       <c r="I18" s="25"/>
       <c r="J18" s="33"/>
@@ -1949,10 +2174,10 @@
         <v>16</v>
       </c>
       <c r="B19" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="25" t="s">
         <v>79</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>86</v>
       </c>
       <c r="D19" s="25" t="s">
         <v>29</v>
@@ -1968,11 +2193,11 @@
         <v>41089</v>
       </c>
       <c r="H19" s="28" t="s">
-        <v>185</v>
+        <v>154</v>
       </c>
       <c r="I19" s="25"/>
       <c r="J19" s="33" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1980,10 +2205,10 @@
         <v>17</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D20" s="25" t="s">
         <v>26</v>
@@ -1999,11 +2224,11 @@
         <v>41089</v>
       </c>
       <c r="H20" s="28" t="s">
-        <v>186</v>
+        <v>155</v>
       </c>
       <c r="I20" s="25"/>
       <c r="J20" s="33" t="s">
-        <v>209</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2011,10 +2236,10 @@
         <v>18</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D21" s="25" t="s">
         <v>37</v>
@@ -2028,11 +2253,11 @@
         <v>40987</v>
       </c>
       <c r="H21" s="28" t="s">
-        <v>187</v>
+        <v>156</v>
       </c>
       <c r="I21" s="25"/>
       <c r="J21" s="33" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2040,10 +2265,10 @@
         <v>19</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D22" s="25" t="s">
         <v>37</v>
@@ -2059,13 +2284,13 @@
         <v>41089</v>
       </c>
       <c r="H22" s="28" t="s">
-        <v>188</v>
+        <v>157</v>
       </c>
       <c r="I22" s="25" t="s">
-        <v>198</v>
+        <v>167</v>
       </c>
       <c r="J22" s="33" t="s">
-        <v>210</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2073,10 +2298,10 @@
         <v>20</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D23" s="25" t="s">
         <v>38</v>
@@ -2092,13 +2317,13 @@
         <v>41183</v>
       </c>
       <c r="H23" s="28" t="s">
-        <v>189</v>
+        <v>158</v>
       </c>
       <c r="I23" s="25" t="s">
-        <v>199</v>
+        <v>168</v>
       </c>
       <c r="J23" s="33" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2106,10 +2331,10 @@
         <v>21</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D24" s="25" t="s">
         <v>40</v>
@@ -2123,11 +2348,11 @@
         <v>40987</v>
       </c>
       <c r="H24" s="28" t="s">
-        <v>190</v>
+        <v>159</v>
       </c>
       <c r="I24" s="25"/>
       <c r="J24" s="33" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2135,10 +2360,10 @@
         <v>22</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D25" s="25" t="s">
         <v>45</v>
@@ -2154,13 +2379,13 @@
         <v>41089</v>
       </c>
       <c r="H25" s="28" t="s">
-        <v>191</v>
+        <v>160</v>
       </c>
       <c r="I25" s="25" t="s">
-        <v>197</v>
+        <v>166</v>
       </c>
       <c r="J25" s="33" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2168,10 +2393,10 @@
         <v>23</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D26" s="25" t="s">
         <v>30</v>
@@ -2187,11 +2412,11 @@
         <v>41160</v>
       </c>
       <c r="H26" s="28" t="s">
-        <v>192</v>
+        <v>161</v>
       </c>
       <c r="I26" s="25"/>
       <c r="J26" s="33" t="s">
-        <v>211</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2199,10 +2424,10 @@
         <v>24</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D27" s="25" t="s">
         <v>27</v>
@@ -2218,11 +2443,11 @@
         <v>41160</v>
       </c>
       <c r="H27" s="28" t="s">
-        <v>193</v>
+        <v>162</v>
       </c>
       <c r="I27" s="25"/>
       <c r="J27" s="33" t="s">
-        <v>212</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2230,10 +2455,10 @@
         <v>25</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D28" s="25" t="s">
         <v>32</v>
@@ -2249,13 +2474,13 @@
         <v>41136</v>
       </c>
       <c r="H28" s="28" t="s">
-        <v>194</v>
+        <v>163</v>
       </c>
       <c r="I28" s="25" t="s">
-        <v>204</v>
+        <v>173</v>
       </c>
       <c r="J28" s="33" t="s">
-        <v>213</v>
+        <v>182</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -2308,10 +2533,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AG33"/>
+  <dimension ref="A2:AG19"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2333,47 +2558,47 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="M2" s="43" t="s">
+      <c r="M2" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="M3" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="N3" s="42"/>
-      <c r="O3" s="42"/>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="42"/>
+      <c r="M3" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="P4" s="4"/>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="M5" s="44" t="s">
+      <c r="M5" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="N5" s="44"/>
-      <c r="O5" s="44"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="44"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="49"/>
+      <c r="R5" s="49"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="M6" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="N6" s="42"/>
-      <c r="O6" s="42"/>
-      <c r="P6" s="42"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="42"/>
+      <c r="M6" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
+      <c r="P6" s="39"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="39"/>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="N7" s="3"/>
@@ -2414,171 +2639,171 @@
       <c r="AF8" s="9"/>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="52" t="s">
+      <c r="F9" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="52"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52"/>
-      <c r="K9" s="52" t="s">
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="K9" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52"/>
-      <c r="N9" s="52"/>
-      <c r="Q9" s="52" t="s">
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="Q9" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="R9" s="52"/>
-      <c r="S9" s="52"/>
-      <c r="T9" s="52"/>
-      <c r="V9" s="52" t="s">
+      <c r="R9" s="37"/>
+      <c r="S9" s="37"/>
+      <c r="T9" s="37"/>
+      <c r="V9" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="W9" s="52"/>
-      <c r="X9" s="52"/>
-      <c r="Y9" s="52"/>
-      <c r="AA9" s="52" t="s">
+      <c r="W9" s="37"/>
+      <c r="X9" s="37"/>
+      <c r="Y9" s="37"/>
+      <c r="AA9" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="AB9" s="52"/>
-      <c r="AC9" s="52"/>
-      <c r="AD9" s="52"/>
-      <c r="AF9" s="46" t="s">
-        <v>172</v>
-      </c>
-      <c r="AG9" s="46"/>
+      <c r="AB9" s="37"/>
+      <c r="AC9" s="37"/>
+      <c r="AD9" s="37"/>
+      <c r="AF9" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="AG9" s="44"/>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="F10" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="F10" s="42" t="s">
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="K10" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="Q10" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="R10" s="39"/>
+      <c r="S10" s="39"/>
+      <c r="T10" s="39"/>
+      <c r="V10" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="W10" s="39"/>
+      <c r="X10" s="39"/>
+      <c r="Y10" s="39"/>
+      <c r="AA10" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB10" s="39"/>
+      <c r="AC10" s="39"/>
+      <c r="AD10" s="39"/>
+      <c r="AF10" s="45"/>
+      <c r="AG10" s="45"/>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="F11" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="K11" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="L11" s="41"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="41"/>
+      <c r="Q11" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="R11" s="41"/>
+      <c r="S11" s="41"/>
+      <c r="T11" s="41"/>
+      <c r="V11" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="W11" s="41"/>
+      <c r="X11" s="41"/>
+      <c r="Y11" s="41"/>
+      <c r="AA11" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB11" s="41"/>
+      <c r="AC11" s="41"/>
+      <c r="AD11" s="41"/>
+      <c r="AF11" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="47"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="F12" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="K10" s="42" t="s">
-        <v>108</v>
-      </c>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="42"/>
-      <c r="Q10" s="42" t="s">
-        <v>117</v>
-      </c>
-      <c r="R10" s="42"/>
-      <c r="S10" s="42"/>
-      <c r="T10" s="42"/>
-      <c r="V10" s="42" t="s">
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="K12" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="L12" s="41"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="Q12" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="R12" s="41"/>
+      <c r="S12" s="41"/>
+      <c r="T12" s="41"/>
+      <c r="V12" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="W12" s="41"/>
+      <c r="X12" s="41"/>
+      <c r="Y12" s="41"/>
+      <c r="AA12" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="W10" s="42"/>
-      <c r="X10" s="42"/>
-      <c r="Y10" s="42"/>
-      <c r="AA10" s="42" t="s">
-        <v>122</v>
-      </c>
-      <c r="AB10" s="42"/>
-      <c r="AC10" s="42"/>
-      <c r="AD10" s="42"/>
-      <c r="AF10" s="47"/>
-      <c r="AG10" s="47"/>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="F11" s="45" t="s">
-        <v>118</v>
-      </c>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
-      <c r="K11" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="L11" s="45"/>
-      <c r="M11" s="45"/>
-      <c r="N11" s="45"/>
-      <c r="Q11" s="45" t="s">
-        <v>124</v>
-      </c>
-      <c r="R11" s="45"/>
-      <c r="S11" s="45"/>
-      <c r="T11" s="45"/>
-      <c r="V11" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="W11" s="45"/>
-      <c r="X11" s="45"/>
-      <c r="Y11" s="45"/>
-      <c r="AA11" s="45" t="s">
-        <v>126</v>
-      </c>
-      <c r="AB11" s="45"/>
-      <c r="AC11" s="45"/>
-      <c r="AD11" s="45"/>
-      <c r="AF11" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG11" s="39"/>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
-        <v>125</v>
-      </c>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="F12" s="45" t="s">
-        <v>121</v>
-      </c>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
-      <c r="K12" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="L12" s="45"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45"/>
-      <c r="Q12" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="R12" s="45"/>
-      <c r="S12" s="45"/>
-      <c r="T12" s="45"/>
-      <c r="V12" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="W12" s="45"/>
-      <c r="X12" s="45"/>
-      <c r="Y12" s="45"/>
-      <c r="AA12" s="45" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB12" s="45"/>
-      <c r="AC12" s="45"/>
-      <c r="AD12" s="45"/>
-      <c r="AF12" s="38" t="s">
+      <c r="AB12" s="41"/>
+      <c r="AC12" s="41"/>
+      <c r="AD12" s="41"/>
+      <c r="AF12" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="AG12" s="39"/>
+      <c r="AG12" s="47"/>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
@@ -2601,16 +2826,16 @@
       <c r="W13" s="23"/>
       <c r="X13" s="6"/>
       <c r="Y13" s="14"/>
-      <c r="AA13" s="45" t="s">
-        <v>123</v>
-      </c>
-      <c r="AB13" s="45"/>
-      <c r="AC13" s="45"/>
-      <c r="AD13" s="45"/>
-      <c r="AF13" s="38" t="s">
+      <c r="AA13" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB13" s="41"/>
+      <c r="AC13" s="41"/>
+      <c r="AD13" s="41"/>
+      <c r="AF13" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="AG13" s="39"/>
+      <c r="AG13" s="47"/>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="C14" s="10"/>
@@ -2619,10 +2844,10 @@
       <c r="S14" s="10"/>
       <c r="X14" s="10"/>
       <c r="AC14" s="10"/>
-      <c r="AF14" s="38" t="s">
+      <c r="AF14" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="AG14" s="39"/>
+      <c r="AG14" s="47"/>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
@@ -2637,299 +2862,264 @@
       <c r="X15" s="9"/>
       <c r="AB15" s="6"/>
       <c r="AC15" s="9"/>
-      <c r="AF15" s="38" t="s">
+      <c r="AF15" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="AG15" s="39"/>
+      <c r="AG15" s="47"/>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A16" s="50" t="s">
+      <c r="A16" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="50"/>
-      <c r="C16" s="51" t="s">
+      <c r="B16" s="40"/>
+      <c r="C16" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="51"/>
-      <c r="F16" s="50" t="s">
+      <c r="D16" s="38"/>
+      <c r="F16" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="50"/>
-      <c r="H16" s="51" t="s">
+      <c r="G16" s="40"/>
+      <c r="H16" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="51"/>
-      <c r="K16" s="50" t="s">
+      <c r="I16" s="38"/>
+      <c r="K16" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="L16" s="50"/>
-      <c r="M16" s="51" t="s">
+      <c r="L16" s="40"/>
+      <c r="M16" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="N16" s="51"/>
-      <c r="Q16" s="50" t="s">
+      <c r="N16" s="38"/>
+      <c r="Q16" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="R16" s="50"/>
-      <c r="S16" s="51" t="s">
+      <c r="R16" s="40"/>
+      <c r="S16" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="T16" s="51"/>
-      <c r="V16" s="50" t="s">
+      <c r="T16" s="38"/>
+      <c r="V16" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="W16" s="50"/>
-      <c r="X16" s="51" t="s">
+      <c r="W16" s="40"/>
+      <c r="X16" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="Y16" s="51"/>
-      <c r="AA16" s="50" t="s">
+      <c r="Y16" s="38"/>
+      <c r="AA16" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="AB16" s="50"/>
-      <c r="AC16" s="51" t="s">
+      <c r="AB16" s="40"/>
+      <c r="AC16" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="AD16" s="51"/>
-      <c r="AF16" s="38" t="s">
+      <c r="AD16" s="38"/>
+      <c r="AF16" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="AG16" s="39"/>
+      <c r="AG16" s="47"/>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A17" s="40" t="s">
-        <v>160</v>
-      </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="36" t="s">
-        <v>161</v>
-      </c>
-      <c r="D17" s="37"/>
-      <c r="F17" s="40" t="s">
-        <v>171</v>
-      </c>
-      <c r="G17" s="41"/>
-      <c r="H17" s="36" t="s">
-        <v>162</v>
-      </c>
-      <c r="I17" s="37"/>
-      <c r="K17" s="40" t="s">
-        <v>163</v>
-      </c>
-      <c r="L17" s="41"/>
-      <c r="M17" s="36" t="s">
-        <v>164</v>
-      </c>
-      <c r="N17" s="37"/>
-      <c r="Q17" s="40" t="s">
-        <v>165</v>
-      </c>
-      <c r="R17" s="41"/>
-      <c r="S17" s="36" t="s">
-        <v>166</v>
-      </c>
-      <c r="T17" s="37"/>
-      <c r="V17" s="40" t="s">
-        <v>167</v>
-      </c>
-      <c r="W17" s="41"/>
-      <c r="X17" s="36" t="s">
-        <v>168</v>
-      </c>
-      <c r="Y17" s="37"/>
-      <c r="AA17" s="40" t="s">
-        <v>169</v>
-      </c>
-      <c r="AB17" s="41"/>
-      <c r="AC17" s="36" t="s">
-        <v>170</v>
-      </c>
-      <c r="AD17" s="37"/>
-      <c r="AF17" s="38" t="s">
+      <c r="A17" s="50" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17" s="51"/>
+      <c r="C17" s="52" t="s">
+        <v>130</v>
+      </c>
+      <c r="D17" s="53"/>
+      <c r="F17" s="50" t="s">
+        <v>140</v>
+      </c>
+      <c r="G17" s="51"/>
+      <c r="H17" s="52" t="s">
+        <v>131</v>
+      </c>
+      <c r="I17" s="53"/>
+      <c r="K17" s="50" t="s">
+        <v>132</v>
+      </c>
+      <c r="L17" s="51"/>
+      <c r="M17" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="N17" s="53"/>
+      <c r="Q17" s="50" t="s">
+        <v>134</v>
+      </c>
+      <c r="R17" s="51"/>
+      <c r="S17" s="52" t="s">
+        <v>135</v>
+      </c>
+      <c r="T17" s="53"/>
+      <c r="V17" s="50" t="s">
+        <v>136</v>
+      </c>
+      <c r="W17" s="51"/>
+      <c r="X17" s="52" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y17" s="53"/>
+      <c r="AA17" s="50" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB17" s="51"/>
+      <c r="AC17" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD17" s="53"/>
+      <c r="AF17" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="AG17" s="39"/>
-    </row>
-    <row r="18" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="48" t="s">
-        <v>128</v>
-      </c>
-      <c r="B18" s="49"/>
-      <c r="C18" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="D18" s="49"/>
-      <c r="F18" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="G18" s="42"/>
-      <c r="H18" s="48" t="s">
-        <v>134</v>
-      </c>
-      <c r="I18" s="49"/>
-      <c r="K18" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="L18" s="49"/>
-      <c r="M18" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="N18" s="49"/>
-      <c r="Q18" s="48" t="s">
-        <v>140</v>
-      </c>
-      <c r="R18" s="49"/>
-      <c r="S18" s="48" t="s">
-        <v>142</v>
-      </c>
-      <c r="T18" s="49"/>
-      <c r="V18" s="48" t="s">
-        <v>144</v>
-      </c>
-      <c r="W18" s="49"/>
-      <c r="X18" s="48" t="s">
-        <v>146</v>
-      </c>
-      <c r="Y18" s="49"/>
-      <c r="AA18" s="48" t="s">
-        <v>149</v>
-      </c>
-      <c r="AB18" s="49"/>
-      <c r="AC18" s="42" t="s">
-        <v>151</v>
-      </c>
-      <c r="AD18" s="42"/>
-    </row>
-    <row r="19" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
-        <v>129</v>
-      </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45" t="s">
-        <v>131</v>
-      </c>
-      <c r="D19" s="45"/>
-      <c r="F19" s="45" t="s">
-        <v>133</v>
-      </c>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="I19" s="45"/>
-      <c r="K19" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="L19" s="45"/>
-      <c r="M19" s="45" t="s">
-        <v>139</v>
-      </c>
-      <c r="N19" s="45"/>
-      <c r="Q19" s="45" t="s">
-        <v>141</v>
-      </c>
-      <c r="R19" s="45"/>
-      <c r="S19" s="45" t="s">
-        <v>143</v>
-      </c>
-      <c r="T19" s="45"/>
-      <c r="V19" s="45" t="s">
-        <v>145</v>
-      </c>
-      <c r="W19" s="45"/>
-      <c r="X19" s="45" t="s">
-        <v>147</v>
-      </c>
-      <c r="Y19" s="45"/>
-      <c r="AA19" s="45" t="s">
-        <v>150</v>
-      </c>
-      <c r="AB19" s="45"/>
-      <c r="AC19" s="45" t="s">
-        <v>152</v>
-      </c>
-      <c r="AD19" s="45"/>
-    </row>
-    <row r="20" spans="1:33" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:33" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:33" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:33" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:33" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:33" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:33" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D28" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D32" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D33" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="AG17" s="47"/>
+    </row>
+    <row r="18" spans="1:33" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="67" t="s">
+        <v>215</v>
+      </c>
+      <c r="B18" s="68"/>
+      <c r="C18" s="67" t="s">
+        <v>217</v>
+      </c>
+      <c r="D18" s="68"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="73" t="s">
+        <v>219</v>
+      </c>
+      <c r="G18" s="70"/>
+      <c r="H18" s="67" t="s">
+        <v>221</v>
+      </c>
+      <c r="I18" s="68"/>
+      <c r="J18" s="69"/>
+      <c r="K18" s="67" t="s">
+        <v>224</v>
+      </c>
+      <c r="L18" s="68"/>
+      <c r="M18" s="67" t="s">
+        <v>225</v>
+      </c>
+      <c r="N18" s="68"/>
+      <c r="O18" s="69"/>
+      <c r="P18" s="69"/>
+      <c r="Q18" s="67" t="s">
+        <v>228</v>
+      </c>
+      <c r="R18" s="68"/>
+      <c r="S18" s="67" t="s">
+        <v>231</v>
+      </c>
+      <c r="T18" s="68"/>
+      <c r="U18" s="69"/>
+      <c r="V18" s="67" t="s">
+        <v>232</v>
+      </c>
+      <c r="W18" s="68"/>
+      <c r="X18" s="67" t="s">
+        <v>234</v>
+      </c>
+      <c r="Y18" s="68"/>
+      <c r="Z18" s="69"/>
+      <c r="AA18" s="67" t="s">
+        <v>223</v>
+      </c>
+      <c r="AB18" s="68"/>
+      <c r="AC18" s="73" t="s">
+        <v>238</v>
+      </c>
+      <c r="AD18" s="70"/>
+    </row>
+    <row r="19" spans="1:33" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="71" t="s">
+        <v>216</v>
+      </c>
+      <c r="B19" s="72"/>
+      <c r="C19" s="71" t="s">
+        <v>218</v>
+      </c>
+      <c r="D19" s="72"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="71" t="s">
+        <v>220</v>
+      </c>
+      <c r="G19" s="72"/>
+      <c r="H19" s="71" t="s">
+        <v>222</v>
+      </c>
+      <c r="I19" s="72"/>
+      <c r="J19" s="69"/>
+      <c r="K19" s="71" t="s">
+        <v>227</v>
+      </c>
+      <c r="L19" s="72"/>
+      <c r="M19" s="71" t="s">
+        <v>226</v>
+      </c>
+      <c r="N19" s="72"/>
+      <c r="O19" s="69"/>
+      <c r="P19" s="69"/>
+      <c r="Q19" s="71" t="s">
+        <v>229</v>
+      </c>
+      <c r="R19" s="72"/>
+      <c r="S19" s="71" t="s">
+        <v>230</v>
+      </c>
+      <c r="T19" s="72"/>
+      <c r="U19" s="69"/>
+      <c r="V19" s="71" t="s">
+        <v>233</v>
+      </c>
+      <c r="W19" s="72"/>
+      <c r="X19" s="71" t="s">
+        <v>235</v>
+      </c>
+      <c r="Y19" s="72"/>
+      <c r="Z19" s="69"/>
+      <c r="AA19" s="71" t="s">
+        <v>236</v>
+      </c>
+      <c r="AB19" s="72"/>
+      <c r="AC19" s="71" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD19" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="Q9:T9"/>
-    <mergeCell ref="V9:Y9"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="Q10:T10"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="Q19:R19"/>
-    <mergeCell ref="V19:W19"/>
-    <mergeCell ref="X19:Y19"/>
-    <mergeCell ref="AA18:AB18"/>
-    <mergeCell ref="AC18:AD18"/>
-    <mergeCell ref="AA19:AB19"/>
-    <mergeCell ref="AC19:AD19"/>
+    <mergeCell ref="AA17:AB17"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="AA11:AD11"/>
+    <mergeCell ref="AA12:AD12"/>
+    <mergeCell ref="AA13:AD13"/>
+    <mergeCell ref="V11:Y11"/>
+    <mergeCell ref="AC17:AD17"/>
+    <mergeCell ref="X17:Y17"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="V17:W17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="AF16:AG16"/>
+    <mergeCell ref="V10:Y10"/>
+    <mergeCell ref="AA10:AD10"/>
+    <mergeCell ref="M2:R2"/>
+    <mergeCell ref="M3:R3"/>
+    <mergeCell ref="M5:R5"/>
+    <mergeCell ref="M6:R6"/>
+    <mergeCell ref="AF11:AG11"/>
+    <mergeCell ref="AF12:AG12"/>
+    <mergeCell ref="AF13:AG13"/>
+    <mergeCell ref="AF14:AG14"/>
     <mergeCell ref="AF9:AG10"/>
     <mergeCell ref="V18:W18"/>
     <mergeCell ref="X18:Y18"/>
@@ -2946,39 +3136,44 @@
     <mergeCell ref="Q12:T12"/>
     <mergeCell ref="AF17:AG17"/>
     <mergeCell ref="AF15:AG15"/>
-    <mergeCell ref="AF16:AG16"/>
-    <mergeCell ref="V10:Y10"/>
-    <mergeCell ref="AA10:AD10"/>
-    <mergeCell ref="M2:R2"/>
-    <mergeCell ref="M3:R3"/>
-    <mergeCell ref="M5:R5"/>
-    <mergeCell ref="M6:R6"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="V17:W17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="AF11:AG11"/>
-    <mergeCell ref="AF12:AG12"/>
-    <mergeCell ref="AF13:AG13"/>
-    <mergeCell ref="AF14:AG14"/>
-    <mergeCell ref="AA17:AB17"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="X19:Y19"/>
+    <mergeCell ref="AA18:AB18"/>
+    <mergeCell ref="AC18:AD18"/>
+    <mergeCell ref="AA19:AB19"/>
+    <mergeCell ref="AC19:AD19"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="Q10:T10"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="K16:L16"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A12:D12"/>
-    <mergeCell ref="AA11:AD11"/>
-    <mergeCell ref="AA12:AD12"/>
-    <mergeCell ref="AA13:AD13"/>
-    <mergeCell ref="V11:Y11"/>
-    <mergeCell ref="AC17:AD17"/>
-    <mergeCell ref="X17:Y17"/>
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="Q9:T9"/>
+    <mergeCell ref="V9:Y9"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A10:D12 F10:I12 K10:N12 Q10:T12 V10:Y12 AA10:AD13 M3 M6">
@@ -2998,7 +3193,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C7"/>
+      <selection activeCell="C8" sqref="C8:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3021,286 +3216,280 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="56" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" s="53" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="54" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="54"/>
+      <c r="A3" s="56"/>
       <c r="B3" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="53"/>
+        <v>101</v>
+      </c>
+      <c r="C3" s="54"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="54"/>
+      <c r="A4" s="56"/>
       <c r="B4" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="C4" s="53"/>
+        <v>102</v>
+      </c>
+      <c r="C4" s="54"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="54"/>
+      <c r="A5" s="56"/>
       <c r="B5" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="53"/>
+        <v>103</v>
+      </c>
+      <c r="C5" s="54"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="54"/>
+      <c r="A6" s="56"/>
       <c r="B6" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="C6" s="53"/>
+        <v>104</v>
+      </c>
+      <c r="C6" s="54"/>
     </row>
     <row r="7" spans="1:3" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="54"/>
+      <c r="A7" s="56"/>
       <c r="B7" s="17"/>
-      <c r="C7" s="53"/>
+      <c r="C7" s="54"/>
     </row>
     <row r="8" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="57" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C8" s="55" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="56"/>
+      <c r="A9" s="57"/>
       <c r="B9" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C9" s="55"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
+      <c r="A10" s="57"/>
       <c r="B10" s="2" t="s">
-        <v>148</v>
+        <v>121</v>
       </c>
       <c r="C10" s="55"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="56"/>
+      <c r="A11" s="57"/>
       <c r="B11" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C11" s="55"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="56"/>
+      <c r="A12" s="57"/>
       <c r="B12" s="13" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C12" s="55"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="56"/>
+      <c r="A13" s="57"/>
       <c r="B13" s="12"/>
       <c r="C13" s="55"/>
     </row>
     <row r="14" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="56" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="C14" s="53" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="54" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="54"/>
+      <c r="A15" s="56"/>
       <c r="B15" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="C15" s="53"/>
+        <v>101</v>
+      </c>
+      <c r="C15" s="54"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="54"/>
+      <c r="A16" s="56"/>
       <c r="B16" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="C16" s="53"/>
+        <v>104</v>
+      </c>
+      <c r="C16" s="54"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="54"/>
+      <c r="A17" s="56"/>
       <c r="B17" s="17"/>
-      <c r="C17" s="53"/>
+      <c r="C17" s="54"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="56" t="s">
+      <c r="A18" s="57" t="s">
         <v>6</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C18" s="55" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="56"/>
+      <c r="A19" s="57"/>
       <c r="B19" s="2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C19" s="55"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="56"/>
+      <c r="A20" s="57"/>
       <c r="B20" s="2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C20" s="55"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="56"/>
+      <c r="A21" s="57"/>
       <c r="B21" s="11" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C21" s="55"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="56"/>
+      <c r="A22" s="57"/>
       <c r="B22" s="12"/>
       <c r="C22" s="55"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="54" t="s">
+      <c r="A23" s="56" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="C23" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" s="54" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="54"/>
+      <c r="A24" s="56"/>
       <c r="B24" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="C24" s="53"/>
+        <v>116</v>
+      </c>
+      <c r="C24" s="54"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="54"/>
+      <c r="A25" s="56"/>
       <c r="B25" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="C25" s="53"/>
+        <v>117</v>
+      </c>
+      <c r="C25" s="54"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="54"/>
+      <c r="A26" s="56"/>
       <c r="B26" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="C26" s="53"/>
+        <v>118</v>
+      </c>
+      <c r="C26" s="54"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="54"/>
+      <c r="A27" s="56"/>
       <c r="B27" s="17"/>
-      <c r="C27" s="53"/>
+      <c r="C27" s="54"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="56" t="s">
+      <c r="A28" s="57" t="s">
         <v>10</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C28" s="55" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="56"/>
+      <c r="A29" s="57"/>
       <c r="B29" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C29" s="55"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="56"/>
+      <c r="A30" s="57"/>
       <c r="B30" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" s="55"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="57"/>
+      <c r="B31" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="C30" s="55"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="56"/>
-      <c r="B31" s="11" t="s">
-        <v>126</v>
-      </c>
       <c r="C31" s="55"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="56"/>
+      <c r="A32" s="57"/>
       <c r="B32" s="12"/>
       <c r="C32" s="55"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="54" t="s">
+      <c r="A33" s="56" t="s">
         <v>12</v>
       </c>
       <c r="B33" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="54" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="56"/>
+      <c r="B34" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="54"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="56"/>
+      <c r="B35" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35" s="54"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="56"/>
+      <c r="B36" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" s="54"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="56"/>
+      <c r="B37" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="C33" s="53" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="54"/>
-      <c r="B34" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="C34" s="53"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="54"/>
-      <c r="B35" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="C35" s="53"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="54"/>
-      <c r="B36" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="C36" s="53"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="54"/>
-      <c r="B37" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="C37" s="53"/>
+      <c r="C37" s="54"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="54"/>
+      <c r="A38" s="56"/>
       <c r="B38" s="20"/>
-      <c r="C38" s="53"/>
+      <c r="C38" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C2:C7"/>
-    <mergeCell ref="C8:C13"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="C28:C32"/>
-    <mergeCell ref="A28:A32"/>
     <mergeCell ref="C33:C38"/>
     <mergeCell ref="A33:A38"/>
     <mergeCell ref="A14:A17"/>
@@ -3309,6 +3498,12 @@
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="A23:A27"/>
     <mergeCell ref="C23:C27"/>
+    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="C28:C32"/>
+    <mergeCell ref="A28:A32"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B38">
@@ -3318,4 +3513,821 @@
   <pageMargins left="0.1" right="0.1" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="97" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
+        <v>214</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="35">
+        <v>10</v>
+      </c>
+      <c r="B4" s="58" t="s">
+        <v>188</v>
+      </c>
+      <c r="C4" s="58" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4" s="58" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="35">
+        <v>11</v>
+      </c>
+      <c r="B5" s="58" t="s">
+        <v>191</v>
+      </c>
+      <c r="C5" s="58" t="s">
+        <v>191</v>
+      </c>
+      <c r="D5" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="E5" s="58" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="35">
+        <v>12</v>
+      </c>
+      <c r="B6" s="58" t="s">
+        <v>193</v>
+      </c>
+      <c r="C6" s="58" t="s">
+        <v>193</v>
+      </c>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="35">
+        <v>1</v>
+      </c>
+      <c r="B7" s="58" t="s">
+        <v>194</v>
+      </c>
+      <c r="C7" s="58" t="s">
+        <v>195</v>
+      </c>
+      <c r="D7" s="58" t="s">
+        <v>196</v>
+      </c>
+      <c r="E7" s="58"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="35">
+        <v>2</v>
+      </c>
+      <c r="B8" s="58" t="s">
+        <v>197</v>
+      </c>
+      <c r="C8" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="35">
+        <v>3</v>
+      </c>
+      <c r="B9" s="58" t="s">
+        <v>199</v>
+      </c>
+      <c r="C9" s="58" t="s">
+        <v>200</v>
+      </c>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="35">
+        <v>4</v>
+      </c>
+      <c r="B10" s="58" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" s="58" t="s">
+        <v>202</v>
+      </c>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="35">
+        <v>5</v>
+      </c>
+      <c r="B11" s="58" t="s">
+        <v>203</v>
+      </c>
+      <c r="C11" s="58" t="s">
+        <v>204</v>
+      </c>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W23"/>
+  <sheetViews>
+    <sheetView showGridLines="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="8.42578125" style="1" customWidth="1"/>
+    <col min="3" max="37" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
+        <v>213</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="59"/>
+      <c r="B3" s="60" t="s">
+        <v>183</v>
+      </c>
+      <c r="C3" s="64">
+        <v>10</v>
+      </c>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64">
+        <v>11</v>
+      </c>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64">
+        <v>12</v>
+      </c>
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="64"/>
+      <c r="T3" s="64"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="61" t="s">
+        <v>205</v>
+      </c>
+      <c r="B4" s="62"/>
+      <c r="C4" s="63">
+        <v>41186</v>
+      </c>
+      <c r="D4" s="63">
+        <v>41193</v>
+      </c>
+      <c r="E4" s="63">
+        <v>41200</v>
+      </c>
+      <c r="F4" s="63">
+        <v>41207</v>
+      </c>
+      <c r="G4" s="63">
+        <v>41214</v>
+      </c>
+      <c r="H4" s="63">
+        <v>41221</v>
+      </c>
+      <c r="I4" s="63">
+        <v>41228</v>
+      </c>
+      <c r="J4" s="63">
+        <v>41235</v>
+      </c>
+      <c r="K4" s="63">
+        <v>41242</v>
+      </c>
+      <c r="L4" s="63">
+        <v>41249</v>
+      </c>
+      <c r="M4" s="63">
+        <v>41256</v>
+      </c>
+      <c r="N4" s="63">
+        <v>41263</v>
+      </c>
+      <c r="O4" s="63">
+        <v>41270</v>
+      </c>
+      <c r="P4" s="63">
+        <v>41277</v>
+      </c>
+      <c r="Q4" s="63">
+        <v>41284</v>
+      </c>
+      <c r="R4" s="63">
+        <v>41291</v>
+      </c>
+      <c r="S4" s="63">
+        <v>41298</v>
+      </c>
+      <c r="T4" s="63">
+        <v>41305</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="42" t="s">
+        <v>206</v>
+      </c>
+      <c r="B5" s="43"/>
+      <c r="C5" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="S5" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="T5" s="35" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="42" t="s">
+        <v>207</v>
+      </c>
+      <c r="B6" s="43"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="35"/>
+      <c r="P6" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q6" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="R6" s="35"/>
+      <c r="S6" s="35"/>
+      <c r="T6" s="35"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="B7" s="43"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="H7" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
+      <c r="P7" s="35"/>
+      <c r="Q7" s="35"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="35"/>
+      <c r="T7" s="35"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="39" t="s">
+        <v>209</v>
+      </c>
+      <c r="B8" s="39"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="J8" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="K8" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="35"/>
+      <c r="R8" s="35"/>
+      <c r="S8" s="35"/>
+      <c r="T8" s="35"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="39" t="s">
+        <v>210</v>
+      </c>
+      <c r="B9" s="39"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="M9" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="N9" s="35"/>
+      <c r="O9" s="35"/>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="35"/>
+      <c r="S9" s="35"/>
+      <c r="T9" s="35"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="B10" s="39"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="O10" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="35"/>
+      <c r="R10" s="35"/>
+      <c r="S10" s="35"/>
+      <c r="T10" s="35"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="59"/>
+      <c r="B13" s="60" t="s">
+        <v>183</v>
+      </c>
+      <c r="C13" s="64">
+        <v>2</v>
+      </c>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="64">
+        <v>3</v>
+      </c>
+      <c r="H13" s="64"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="64"/>
+      <c r="K13" s="64">
+        <v>4</v>
+      </c>
+      <c r="L13" s="64"/>
+      <c r="M13" s="64"/>
+      <c r="N13" s="64"/>
+      <c r="O13" s="64">
+        <v>5</v>
+      </c>
+      <c r="P13" s="64"/>
+      <c r="Q13" s="64"/>
+      <c r="R13" s="64"/>
+      <c r="S13" s="64"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="61" t="s">
+        <v>205</v>
+      </c>
+      <c r="B14" s="62"/>
+      <c r="C14" s="63">
+        <v>41312</v>
+      </c>
+      <c r="D14" s="63">
+        <v>41319</v>
+      </c>
+      <c r="E14" s="63">
+        <v>41326</v>
+      </c>
+      <c r="F14" s="63">
+        <v>41333</v>
+      </c>
+      <c r="G14" s="63">
+        <v>41340</v>
+      </c>
+      <c r="H14" s="63">
+        <v>41347</v>
+      </c>
+      <c r="I14" s="63">
+        <v>41354</v>
+      </c>
+      <c r="J14" s="63">
+        <v>41361</v>
+      </c>
+      <c r="K14" s="63">
+        <v>41368</v>
+      </c>
+      <c r="L14" s="63">
+        <v>41375</v>
+      </c>
+      <c r="M14" s="63">
+        <v>41382</v>
+      </c>
+      <c r="N14" s="63">
+        <v>41389</v>
+      </c>
+      <c r="O14" s="63">
+        <v>41396</v>
+      </c>
+      <c r="P14" s="63">
+        <v>41403</v>
+      </c>
+      <c r="Q14" s="63">
+        <v>41410</v>
+      </c>
+      <c r="R14" s="63">
+        <v>41417</v>
+      </c>
+      <c r="S14" s="63">
+        <v>41424</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="42" t="s">
+        <v>206</v>
+      </c>
+      <c r="B15" s="43"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="L15" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="M15" s="35"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="35"/>
+      <c r="R15" s="35"/>
+      <c r="S15" s="35"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="42" t="s">
+        <v>207</v>
+      </c>
+      <c r="B16" s="43"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="N16" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="O16" s="35"/>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="35"/>
+      <c r="R16" s="35"/>
+      <c r="S16" s="35"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="B17" s="43"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="F17" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="35"/>
+      <c r="O17" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="P17" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q17" s="35"/>
+      <c r="R17" s="35"/>
+      <c r="S17" s="35"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="39" t="s">
+        <v>209</v>
+      </c>
+      <c r="B18" s="39"/>
+      <c r="C18" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="R18" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="S18" s="35" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="39" t="s">
+        <v>210</v>
+      </c>
+      <c r="B19" s="39"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="J19" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="K19" s="35"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="35"/>
+      <c r="P19" s="35"/>
+      <c r="Q19" s="35"/>
+      <c r="R19" s="35"/>
+      <c r="S19" s="35"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="B20" s="39"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="H20" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="35"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="35"/>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="35"/>
+      <c r="R20" s="35"/>
+      <c r="S20" s="35"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22" s="65"/>
+    </row>
+    <row r="23" spans="1:23" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="74" t="s">
+        <v>239</v>
+      </c>
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="66"/>
+      <c r="J23" s="66"/>
+      <c r="K23" s="66"/>
+      <c r="L23" s="66"/>
+      <c r="M23" s="66"/>
+      <c r="N23" s="66"/>
+      <c r="O23" s="66"/>
+      <c r="P23" s="66"/>
+      <c r="Q23" s="66"/>
+      <c r="R23" s="66"/>
+      <c r="S23" s="66"/>
+      <c r="T23" s="66"/>
+      <c r="U23" s="66"/>
+      <c r="V23" s="66"/>
+      <c r="W23" s="66"/>
+    </row>
+  </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="B23:W23"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="K13:N13"/>
+    <mergeCell ref="O13:S13"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="P3:T3"/>
+    <mergeCell ref="G13:J13"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C5:T10 C15:S20">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="notEqual">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>